<commit_message>
fixing backend to connect to front
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -360,10 +360,10 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="13.44" customWidth="1" style="4" min="1" max="1"/>
     <col width="16.33" customWidth="1" style="4" min="2" max="2"/>
@@ -425,7 +425,7 @@
         <v>154.25</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F2" s="7" t="n">
         <v>20</v>
@@ -451,7 +451,7 @@
         <v>194.17</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F3" s="7" t="n">
         <v>20</v>

</xml_diff>

<commit_message>
FINALLY CONNECTED THE MOST IMPORTANT PART
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -363,7 +363,7 @@
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="13.44" customWidth="1" style="4" min="1" max="1"/>
     <col width="16.33" customWidth="1" style="4" min="2" max="2"/>
@@ -425,7 +425,7 @@
         <v>154.25</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F2" s="7" t="n">
         <v>20</v>
@@ -451,7 +451,7 @@
         <v>194.17</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F3" s="7" t="n">
         <v>20</v>

</xml_diff>

<commit_message>
Fixed non updating total and non clearing treeview in sales
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -424,10 +424,8 @@
       <c r="D2" s="4" t="n">
         <v>154.25</v>
       </c>
-      <c r="E2" s="7" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="E2" s="7" t="n">
+        <v>22</v>
       </c>
       <c r="F2" s="7" t="n">
         <v>20</v>
@@ -507,7 +505,7 @@
         <v>131.5</v>
       </c>
       <c r="E5" s="7" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F5" s="7" t="n">
         <v>10</v>

</xml_diff>